<commit_message>
CotizaciÃ³n: extras en tarifa, logÃ­stica J30+J31-J32, boleta con cod_contract al pasar a COTIZADO, header centrado en plantilla boleta
</commit_message>
<xml_diff>
--- a/public/assets/templates/PLANTILLA_COTIZACION_INICIAL_CALCULADORA.xlsx
+++ b/public/assets/templates/PLANTILLA_COTIZACION_INICIAL_CALCULADORA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Proyectos\Probusiness\intranet_back\public\assets\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\Proyectos\Probusiness\probusiness_intranetv2_back\public\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639EDD23-8386-46E0-ADE4-B3885F67EB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A2571F-A121-4985-8A03-3E0F0E380D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -24,43 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="130">
   <si>
     <t>VALOR UNITARIO</t>
   </si>
@@ -222,9 +191,6 @@
   </si>
   <si>
     <t>NOTAS:</t>
-  </si>
-  <si>
-    <t>TARIFA</t>
   </si>
   <si>
     <t xml:space="preserve"> No se aceptan marcas con medidas  de frontera. </t>
@@ -324,12 +290,6 @@
     <t>NOMBRE:</t>
   </si>
   <si>
-    <t>TIPO DE CLIENTE</t>
-  </si>
-  <si>
-    <t>ANTIGUO</t>
-  </si>
-  <si>
     <t>NUEVO</t>
   </si>
   <si>
@@ -339,25 +299,10 @@
     <t>21.Se emitirá comprobante (boleta o Factura) de su importación en base a la estrategia de declaración realizada.</t>
   </si>
   <si>
-    <t>PILOTO</t>
-  </si>
-  <si>
-    <t>SOCIO</t>
-  </si>
-  <si>
-    <t>DISTRIBUCIÓN</t>
-  </si>
-  <si>
     <t>TOTAL CBM</t>
   </si>
   <si>
-    <t>MANUAL</t>
-  </si>
-  <si>
     <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>Tarifa</t>
   </si>
   <si>
     <r>
@@ -431,24 +376,6 @@
   </si>
   <si>
     <t>FECHA:</t>
-  </si>
-  <si>
-    <t>0-0.59</t>
-  </si>
-  <si>
-    <t>0.59-1</t>
-  </si>
-  <si>
-    <t>1-2.09</t>
-  </si>
-  <si>
-    <t>2.1-3.1</t>
-  </si>
-  <si>
-    <t>3.1-4.1</t>
-  </si>
-  <si>
-    <t>4.1- +</t>
   </si>
   <si>
     <r>
@@ -698,15 +625,6 @@
     <t>TOTALES</t>
   </si>
   <si>
-    <t>TARIFA PRELIMINAR</t>
-  </si>
-  <si>
-    <t>CBM PRELIMINAR</t>
-  </si>
-  <si>
-    <t>TOTAL TARIFA MANUAL</t>
-  </si>
-  <si>
     <t>Servicio de Consolidado antes de la Fecha de Corte 23/01</t>
   </si>
   <si>
@@ -716,40 +634,36 @@
     <t>BASE DE LAMPARA LED</t>
   </si>
   <si>
-    <t>ITEMS ADICIONALES (3)</t>
-  </si>
-  <si>
-    <t>PROVS ADICIONALES (1)</t>
-  </si>
-  <si>
     <t xml:space="preserve">CARGOS EXTRAS (QTY PROVEEDORES O QTY ITEMS) </t>
   </si>
   <si>
     <t>DESCUENTO APLICABLE</t>
+  </si>
+  <si>
+    <t>PRO MUNDO COMEX S.A.C.</t>
+  </si>
+  <si>
+    <t>RUC: 20612452432</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="17">
+  <numFmts count="13">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.000_ ;_-[$$-409]* \-#,##0.000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="167" formatCode="[$$-409]#,##0"/>
     <numFmt numFmtId="168" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="169" formatCode="0.00\ &quot;cm&quot;"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000\ &quot;m3&quot;"/>
-    <numFmt numFmtId="171" formatCode="0.0\ &quot;cm&quot;"/>
-    <numFmt numFmtId="172" formatCode="0.0\ &quot;kg&quot;"/>
-    <numFmt numFmtId="173" formatCode="_-[$S/-280A]\ * #,##0.00_-;\-[$S/-280A]\ * #,##0.00_-;_-[$S/-280A]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="174" formatCode="_-[$$-409]* #,##0.0_ ;_-[$$-409]* \-#,##0.0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="175" formatCode="_-[$$-540A]* #,##0.000_ ;_-[$$-540A]* \-#,##0.000\ ;_-[$$-540A]* &quot;-&quot;???_ ;_-@_ "/>
-    <numFmt numFmtId="176" formatCode="0.00\ &quot;x UC&quot;"/>
-    <numFmt numFmtId="177" formatCode="_-[$$-409]* #,##0.000_ ;_-[$$-409]* \-#,##0.000\ ;_-[$$-409]* &quot;-&quot;???_ ;_-@_ "/>
-    <numFmt numFmtId="178" formatCode="[$$-540A]#,##0.00"/>
-    <numFmt numFmtId="179" formatCode="\$#,##0.00;\-\$#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="#,##0.000\ &quot;m3&quot;"/>
+    <numFmt numFmtId="170" formatCode="0.0\ &quot;cm&quot;"/>
+    <numFmt numFmtId="171" formatCode="0.0\ &quot;kg&quot;"/>
+    <numFmt numFmtId="172" formatCode="_-[$S/-280A]\ * #,##0.00_-;\-[$S/-280A]\ * #,##0.00_-;_-[$S/-280A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="173" formatCode="_-[$$-409]* #,##0.0_ ;_-[$$-409]* \-#,##0.0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="174" formatCode="0.00\ &quot;x UC&quot;"/>
+    <numFmt numFmtId="176" formatCode="\$#,##0.00;\-\$#,##0.00"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -902,12 +816,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="14"/>
@@ -1009,14 +917,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <u/>
       <sz val="12"/>
       <color theme="1"/>
@@ -1041,8 +941,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF500B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1112,18 +1028,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE37C1A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1468,9 +1372,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1581,13 +1485,9 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1615,9 +1515,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1636,7 +1533,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1648,58 +1544,40 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="170" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="27" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="26" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1708,75 +1586,67 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="175" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="33" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="34" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="8" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="8" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="35" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="34" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="35" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="35" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="37" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="37" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1784,43 +1654,58 @@
     <xf numFmtId="14" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="31" fillId="11" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="11" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="31" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="11" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="31" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="31" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="31" fillId="11" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="11" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="31" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="31" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="31" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="31" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="31" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1844,13 +1729,22 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="27" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="26" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1859,56 +1753,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1952,9 +1819,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF500B"/>
       <color rgb="FFDD7105"/>
       <color rgb="FFE37C1A"/>
-      <color rgb="FFFF500B"/>
       <color rgb="FFC87700"/>
       <color rgb="FFFF9900"/>
       <color rgb="FF009999"/>
@@ -1969,10 +1836,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2530,76 +2393,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>17</xdr:col>
-          <xdr:colOff>220980</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>220980</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>18</xdr:col>
-          <xdr:colOff>464820</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>68580</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2049" name="Button 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2049"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="36576" bIns="32004" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Calibri"/>
-                  <a:ea typeface="Calibri"/>
-                  <a:cs typeface="Calibri"/>
-                </a:rPr>
-                <a:t>Botón 1</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -2742,16 +2535,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>587375</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>119783</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>173182</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>878910</xdr:colOff>
+      <xdr:colOff>1337841</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>146069</xdr:rowOff>
+      <xdr:rowOff>172046</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2781,8 +2574,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1063625" y="0"/>
-          <a:ext cx="1212285" cy="1193819"/>
+          <a:off x="1046306" y="173182"/>
+          <a:ext cx="1218058" cy="1202478"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2800,7 +2593,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>464757</xdr:colOff>
+      <xdr:colOff>239621</xdr:colOff>
       <xdr:row>94</xdr:row>
       <xdr:rowOff>33834</xdr:rowOff>
     </xdr:to>
@@ -2841,95 +2634,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1939636</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>124689</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>299035</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>27845</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="CuadroTexto 25">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2895600" y="353289"/>
-          <a:ext cx="3132290" cy="1032301"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-PE" sz="2000" b="1">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>PRO MUNDO COMEX S.A.C.</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="es-PE" sz="2000" b="1">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="es-PE" sz="2000" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FF500B"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>RUC: 20612452432</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-PE" sz="2000" b="0">
-            <a:solidFill>
-              <a:srgbClr val="FF500B"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2939,9 +2643,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>401739</xdr:colOff>
+      <xdr:colOff>280511</xdr:colOff>
       <xdr:row>111</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>177799</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2972,64 +2676,6 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>74083</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Conector recto de flecha 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13631333" y="2423583"/>
-          <a:ext cx="592667" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3297,319 +2943,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="A1:Y109"/>
+  <dimension ref="A1:S109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.88671875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.88671875" style="1"/>
+    <col min="7" max="7" width="4" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18">
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="31"/>
-    </row>
-    <row r="2" spans="1:25" ht="18">
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="31"/>
-    </row>
-    <row r="3" spans="1:25">
-      <c r="F3" s="163"/>
-      <c r="G3" s="163"/>
-      <c r="H3" s="163"/>
-      <c r="I3" s="163"/>
-      <c r="W3" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
-      <c r="H4" s="170"/>
-      <c r="I4" s="170"/>
-      <c r="J4" s="40"/>
-      <c r="W4" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
-      <c r="W5" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="W6" s="82" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
-      <c r="D7" s="171" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="171"/>
-      <c r="F7" s="171"/>
-      <c r="W7" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1"/>
+    <row r="2" spans="1:11" ht="18.75" customHeight="1"/>
+    <row r="3" spans="1:11">
+      <c r="C3" s="115" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+    </row>
+    <row r="5" spans="1:11" ht="26.25">
+      <c r="C5" s="116" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="D7" s="131" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="131"/>
+      <c r="F7" s="131"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="47"/>
-      <c r="D8" s="67" t="s">
+      <c r="D8" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="68" t="s">
+      <c r="E8" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="69"/>
+      <c r="F8" s="66"/>
       <c r="G8" s="31"/>
       <c r="H8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="176">
+      <c r="I8" s="134">
         <f>+'2'!D5</f>
         <v>1</v>
       </c>
-      <c r="J8" s="176"/>
-      <c r="K8" s="176"/>
-      <c r="T8" s="88"/>
-      <c r="W8" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="J8" s="134"/>
+      <c r="K8" s="134"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="33" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B9" s="47"/>
-      <c r="D9" s="70" t="s">
-        <v>102</v>
-      </c>
-      <c r="E9" s="135">
+      <c r="D9" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="117">
         <f ca="1">+TODAY()</f>
-        <v>46053</v>
-      </c>
-      <c r="F9" s="136"/>
+        <v>46055</v>
+      </c>
+      <c r="F9" s="118"/>
       <c r="G9" s="31"/>
       <c r="H9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="177">
+      <c r="I9" s="135">
         <f>+'2'!D6</f>
         <v>23.2</v>
       </c>
-      <c r="J9" s="177"/>
-      <c r="K9" s="177"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="113" t="s">
-        <v>88</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25">
+      <c r="J9" s="135"/>
+      <c r="K9" s="135"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="33" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B10" s="47"/>
-      <c r="D10" s="78" t="s">
+      <c r="D10" s="74" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="77"/>
+      <c r="F10" s="73"/>
       <c r="G10" s="31"/>
       <c r="H10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10" s="91">
+        <v>72</v>
+      </c>
+      <c r="I10" s="80">
         <v>0</v>
       </c>
-      <c r="J10" s="91">
+      <c r="J10" s="80">
         <v>0</v>
       </c>
-      <c r="K10" s="91">
+      <c r="K10" s="80">
         <v>0</v>
       </c>
-      <c r="R10" s="81" t="s">
-        <v>82</v>
-      </c>
-      <c r="S10" s="50" cm="1">
-        <f t="array" ref="S10">IF('1'!$I$11&lt;0.59,280,IF('1'!$I$11&lt;1,375,IF('1'!$I$11&lt;=2.09,375*'1'!$I$11,IF('1'!$I$11&lt;=3.09,350*'1'!$I$11,IF('1'!$I$11&lt;=4.09,325*'1'!$I$11,IF('1'!$I$11&gt;4.09,300*'1'!$I$11,ERROR))))))</f>
-        <v>280</v>
-      </c>
-      <c r="T10" s="85">
-        <f>IF($I$11&lt;1,S10,S10/$I$11)</f>
-        <v>280</v>
-      </c>
-      <c r="U10" s="49"/>
-      <c r="V10" s="81"/>
-      <c r="W10" s="81" t="s">
-        <v>82</v>
-      </c>
-      <c r="X10" s="81" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y10" s="81" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25">
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="D11" s="71" t="s">
+      <c r="B11" s="53"/>
+      <c r="D11" s="68" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="72"/>
+        <v>79</v>
+      </c>
+      <c r="F11" s="69"/>
       <c r="H11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="173">
+      <c r="I11" s="132">
         <f>+'2'!D8</f>
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="J11" s="173"/>
-      <c r="K11" s="173"/>
-      <c r="L11" s="62"/>
-      <c r="R11" s="81" t="s">
-        <v>81</v>
-      </c>
-      <c r="S11" s="50" cm="1">
-        <f t="array" ref="S11">IF('1'!$I$11&lt;0.59,260,IF('1'!$I$11&lt;1,350,IF('1'!$I$11&lt;2.09,350*'1'!$I$11,IF('1'!$I$11&lt;3.09,325*'1'!$I$11,IF('1'!$I$11&lt;4.09,'1'!$I$11*300,IF('1'!$I$11&gt;4.09,280*'1'!$I$11,ERROR))))))</f>
-        <v>260</v>
-      </c>
-      <c r="T11" s="85">
-        <f>IF($I$11&lt;1,S11,S11/$I$11)</f>
-        <v>260</v>
-      </c>
-      <c r="U11" s="3"/>
-      <c r="V11" s="81" t="s">
-        <v>103</v>
-      </c>
-      <c r="W11" s="81">
-        <v>280</v>
-      </c>
-      <c r="X11" s="81">
-        <v>260</v>
-      </c>
-      <c r="Y11" s="134">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25">
-      <c r="R12" s="81" t="s">
-        <v>89</v>
-      </c>
-      <c r="S12" s="112">
-        <f>+P22</f>
-        <v>685</v>
-      </c>
-      <c r="T12" s="85">
-        <f>IF($I$11&lt;1,S12,S12/$I$11)</f>
-        <v>685</v>
-      </c>
-      <c r="U12" s="3"/>
-      <c r="V12" s="81" t="s">
-        <v>104</v>
-      </c>
-      <c r="W12" s="81">
-        <v>375</v>
-      </c>
-      <c r="X12" s="81">
-        <v>350</v>
-      </c>
-      <c r="Y12" s="134"/>
-    </row>
-    <row r="13" spans="1:25">
-      <c r="A13" s="175" t="s">
+      <c r="J11" s="132"/>
+      <c r="K11" s="132"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="175"/>
-      <c r="C13" s="175"/>
-      <c r="D13" s="175"/>
-      <c r="E13" s="175"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
+      <c r="B13" s="133"/>
+      <c r="C13" s="133"/>
+      <c r="D13" s="133"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
       <c r="J13" s="36" t="s">
         <v>34</v>
       </c>
       <c r="K13" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="R13" s="81" t="s">
-        <v>86</v>
-      </c>
-      <c r="S13" s="50">
-        <f>IF('1'!$I$11&lt;1,250,IF('1'!$I$11&lt;4,250*'1'!$I$11,IF('1'!$I$11&lt;=10,250*'1'!$I$11,IF('1'!$I$11&gt;10,250*'1'!$I$11,"VERIFICA EL CBM"))))</f>
-        <v>250</v>
-      </c>
-      <c r="T13" s="85">
-        <f>IF($I$11&lt;1,S13,S13/$I$11)</f>
-        <v>250</v>
-      </c>
-      <c r="U13" s="87"/>
-      <c r="V13" s="100" t="s">
-        <v>105</v>
-      </c>
-      <c r="W13" s="100">
-        <v>375</v>
-      </c>
-      <c r="X13" s="81">
-        <v>350</v>
-      </c>
-      <c r="Y13" s="134"/>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="A14" s="151" t="s">
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="138" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="151"/>
-      <c r="C14" s="151"/>
+      <c r="B14" s="138"/>
+      <c r="C14" s="138"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
@@ -3621,59 +3141,28 @@
       <c r="K14" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="R14" s="81" t="s">
-        <v>85</v>
-      </c>
-      <c r="S14" s="50">
-        <f>IF('1'!$I$11&lt;1,250,250*'1'!$I$11)</f>
-        <v>250</v>
-      </c>
-      <c r="T14" s="85">
-        <f>IF($I$11&lt;1,S14,S14/$I$11)</f>
-        <v>250</v>
-      </c>
-      <c r="V14" s="100" t="s">
-        <v>106</v>
-      </c>
-      <c r="W14" s="100">
-        <v>350</v>
-      </c>
-      <c r="X14" s="81">
-        <v>325</v>
-      </c>
-      <c r="Y14" s="134"/>
-    </row>
-    <row r="15" spans="1:25">
-      <c r="A15" s="150" t="s">
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="150"/>
-      <c r="C15" s="150"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="137"/>
       <c r="D15" s="38"/>
       <c r="E15" s="38"/>
       <c r="F15" s="38"/>
       <c r="G15" s="38"/>
       <c r="H15" s="38"/>
       <c r="I15" s="38"/>
-      <c r="J15" s="46">
-        <f>IF(I11&lt;1,'2'!D21+'2'!D24,60%*(T16*I11)+'2'!D24)</f>
-        <v>461</v>
+      <c r="J15" s="46" t="e">
+        <f>IF(I11&lt;1,'2'!D21+'2'!D24,60%*(#REF!*I11)+'2'!D24)</f>
+        <v>#REF!</v>
       </c>
       <c r="K15" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="V15" s="81" t="s">
-        <v>107</v>
-      </c>
-      <c r="W15" s="81">
-        <v>325</v>
-      </c>
-      <c r="X15" s="81">
-        <v>300</v>
-      </c>
-      <c r="Y15" s="134"/>
-    </row>
-    <row r="16" spans="1:25">
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
@@ -3685,37 +3174,15 @@
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
-      <c r="J16" s="45">
+      <c r="J16" s="45" t="e">
         <f>SUM(J14:J15)</f>
-        <v>1681</v>
+        <v>#REF!</v>
       </c>
       <c r="K16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="O16" s="49"/>
-      <c r="R16" s="81" t="s">
-        <v>91</v>
-      </c>
-      <c r="S16" s="81" t="str">
-        <f>E11</f>
-        <v>NUEVO</v>
-      </c>
-      <c r="T16" s="81">
-        <f>VLOOKUP(S16,R10:T14,3,0)</f>
-        <v>280</v>
-      </c>
-      <c r="V16" s="81" t="s">
-        <v>108</v>
-      </c>
-      <c r="W16" s="81">
-        <v>300</v>
-      </c>
-      <c r="X16" s="81">
-        <v>280</v>
-      </c>
-      <c r="Y16" s="134"/>
-    </row>
-    <row r="17" spans="1:16">
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="31"/>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
@@ -3727,9 +3194,8 @@
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
-      <c r="O17" s="49"/>
-    </row>
-    <row r="18" spans="1:16">
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="31"/>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
@@ -3741,22 +3207,18 @@
       <c r="I18" s="31"/>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
-      <c r="O18" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="175" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="175"/>
-      <c r="C19" s="175"/>
-      <c r="D19" s="175"/>
-      <c r="E19" s="175"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="133" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="133"/>
+      <c r="C19" s="133"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
       <c r="I19" s="36" t="s">
         <v>42</v>
       </c>
@@ -3766,14 +3228,8 @@
       <c r="K19" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="O19" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="P19" s="5">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="31" t="s">
         <v>37</v>
       </c>
@@ -3784,28 +3240,19 @@
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
       <c r="H20" s="31"/>
-      <c r="I20" s="64">
+      <c r="I20" s="61">
         <f>MAX('2'!C33:C33)</f>
         <v>0</v>
       </c>
-      <c r="J20" s="45">
+      <c r="J20" s="45" t="e">
         <f>'2'!D34</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="K20" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="N20" s="106" t="s">
-        <v>54</v>
-      </c>
-      <c r="O20" s="124" t="s">
-        <v>143</v>
-      </c>
-      <c r="P20" s="124">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="31" t="s">
         <v>38</v>
       </c>
@@ -3816,28 +3263,18 @@
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
-      <c r="I21" s="64">
+      <c r="I21" s="61">
         <v>0.16</v>
       </c>
-      <c r="J21" s="45">
+      <c r="J21" s="45" t="e">
         <f>'2'!D35</f>
-        <v>268.95999999999998</v>
+        <v>#REF!</v>
       </c>
       <c r="K21" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="N21" s="107">
-        <f>J31/I11</f>
-        <v>595.23809523809518</v>
-      </c>
-      <c r="O21" s="125" t="s">
-        <v>144</v>
-      </c>
-      <c r="P21" s="125">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="31" t="s">
         <v>39</v>
       </c>
@@ -3848,25 +3285,18 @@
       <c r="F22" s="31"/>
       <c r="G22" s="31"/>
       <c r="H22" s="31"/>
-      <c r="I22" s="64">
+      <c r="I22" s="61">
         <v>0.02</v>
       </c>
-      <c r="J22" s="45">
+      <c r="J22" s="45" t="e">
         <f>'2'!D36</f>
-        <v>33.619999999999997</v>
+        <v>#REF!</v>
       </c>
       <c r="K22" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="O22" s="120" t="s">
-        <v>139</v>
-      </c>
-      <c r="P22" s="120">
-        <f>+P19+P20+P21</f>
-        <v>685</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="38" t="s">
         <v>40</v>
       </c>
@@ -3877,7 +3307,7 @@
       <c r="F23" s="38"/>
       <c r="G23" s="38"/>
       <c r="H23" s="38"/>
-      <c r="I23" s="80">
+      <c r="I23" s="75">
         <f>MAX('2'!C30:C30)</f>
         <v>0</v>
       </c>
@@ -3889,7 +3319,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:12">
       <c r="A24" s="33" t="s">
         <v>43</v>
       </c>
@@ -3901,20 +3331,15 @@
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
       <c r="I24" s="34"/>
-      <c r="J24" s="45">
+      <c r="J24" s="45" t="e">
         <f>SUM(J20:J23)</f>
-        <v>302.58</v>
+        <v>#REF!</v>
       </c>
       <c r="K24" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="L24" s="79"/>
-      <c r="N24" s="126">
-        <f>J30/I11</f>
-        <v>8154.7619047619046</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="31"/>
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
@@ -3927,7 +3352,7 @@
       <c r="J25" s="37"/>
       <c r="K25" s="34"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:12">
       <c r="A26" s="38" t="s">
         <v>41</v>
       </c>
@@ -3938,18 +3363,18 @@
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
       <c r="H26" s="38"/>
-      <c r="I26" s="65" t="s">
-        <v>74</v>
-      </c>
-      <c r="J26" s="46">
+      <c r="I26" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="J26" s="46" t="e">
         <f>'2'!D37</f>
-        <v>69.425300000000007</v>
+        <v>#REF!</v>
       </c>
       <c r="K26" s="39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:12">
       <c r="A27" s="33" t="s">
         <v>8</v>
       </c>
@@ -3960,40 +3385,36 @@
       <c r="F27" s="31"/>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
-      <c r="J27" s="45">
+      <c r="J27" s="45" t="e">
         <f>J24+J26</f>
-        <v>372.00529999999998</v>
+        <v>#REF!</v>
       </c>
       <c r="K27" s="34" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.6">
-      <c r="A29" s="174" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="174"/>
-      <c r="C29" s="174"/>
-      <c r="D29" s="174"/>
-      <c r="E29" s="174"/>
-      <c r="F29" s="89"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90" t="s">
+    <row r="29" spans="1:12" ht="15.75">
+      <c r="A29" s="145" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="145"/>
+      <c r="C29" s="145"/>
+      <c r="D29" s="145"/>
+      <c r="E29" s="145"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="K29" s="90" t="s">
+      <c r="K29" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="M29" s="79">
-        <f>J30/I11</f>
-        <v>8154.7619047619046</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="31" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B30" s="31"/>
       <c r="C30" s="31"/>
@@ -4003,17 +3424,17 @@
       <c r="G30" s="31"/>
       <c r="H30" s="45"/>
       <c r="I30" s="45"/>
-      <c r="J30" s="45">
+      <c r="J30" s="45" t="e">
         <f>+'2'!D45+'2'!D21</f>
-        <v>685</v>
+        <v>#REF!</v>
       </c>
       <c r="K30" s="34" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:12">
       <c r="A31" s="31" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="B31" s="31"/>
       <c r="C31" s="31"/>
@@ -4029,13 +3450,10 @@
       <c r="K31" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="L31" s="106" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="122" t="s">
-        <v>146</v>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="106" t="s">
+        <v>127</v>
       </c>
       <c r="B32" s="31"/>
       <c r="C32" s="31"/>
@@ -4045,13 +3463,13 @@
       <c r="G32" s="31"/>
       <c r="H32" s="45"/>
       <c r="I32" s="45"/>
-      <c r="J32" s="123">
+      <c r="J32" s="107">
         <v>100</v>
       </c>
       <c r="K32" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="L32" s="106"/>
+      <c r="L32" s="94"/>
     </row>
     <row r="33" spans="1:19">
       <c r="A33" s="38" t="s">
@@ -4065,9 +3483,9 @@
       <c r="G33" s="38"/>
       <c r="H33" s="46"/>
       <c r="I33" s="46"/>
-      <c r="J33" s="46">
+      <c r="J33" s="46" t="e">
         <f>J27</f>
-        <v>372.00529999999998</v>
+        <v>#REF!</v>
       </c>
       <c r="K33" s="39" t="s">
         <v>35</v>
@@ -4076,7 +3494,7 @@
     </row>
     <row r="34" spans="1:19">
       <c r="A34" s="33" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B34" s="31"/>
       <c r="C34" s="31"/>
@@ -4086,20 +3504,20 @@
       <c r="G34" s="31"/>
       <c r="H34" s="45"/>
       <c r="I34" s="45"/>
-      <c r="J34" s="45">
+      <c r="J34" s="45" t="e">
         <f>(J30+J31+J33)-J32</f>
-        <v>1007.0053</v>
+        <v>#REF!</v>
       </c>
       <c r="K34" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="M34" s="139" t="s">
-        <v>121</v>
-      </c>
-      <c r="N34" s="139"/>
-      <c r="O34" s="139"/>
-      <c r="P34" s="139"/>
-      <c r="Q34" s="139"/>
+      <c r="M34" s="121" t="s">
+        <v>107</v>
+      </c>
+      <c r="N34" s="121"/>
+      <c r="O34" s="121"/>
+      <c r="P34" s="121"/>
+      <c r="Q34" s="121"/>
     </row>
     <row r="35" spans="1:19" ht="20.25" customHeight="1">
       <c r="A35" s="33"/>
@@ -4113,118 +3531,118 @@
       <c r="I35" s="37"/>
       <c r="J35" s="37"/>
       <c r="K35" s="34"/>
-      <c r="M35" s="140"/>
-      <c r="N35" s="140"/>
-      <c r="O35" s="140"/>
-      <c r="P35" s="140"/>
-      <c r="Q35" s="140"/>
+      <c r="M35" s="122"/>
+      <c r="N35" s="122"/>
+      <c r="O35" s="122"/>
+      <c r="P35" s="122"/>
+      <c r="Q35" s="122"/>
     </row>
     <row r="36" spans="1:19" ht="15" customHeight="1">
-      <c r="A36" s="154" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36" s="155"/>
-      <c r="C36" s="155"/>
-      <c r="D36" s="155"/>
-      <c r="E36" s="155"/>
-      <c r="F36" s="155"/>
-      <c r="G36" s="155"/>
-      <c r="H36" s="155"/>
-      <c r="I36" s="155"/>
-      <c r="J36" s="155"/>
-      <c r="K36" s="156"/>
-      <c r="M36" s="147" t="s">
+      <c r="A36" s="141" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="142"/>
+      <c r="C36" s="142"/>
+      <c r="D36" s="142"/>
+      <c r="E36" s="142"/>
+      <c r="F36" s="142"/>
+      <c r="G36" s="142"/>
+      <c r="H36" s="142"/>
+      <c r="I36" s="142"/>
+      <c r="J36" s="142"/>
+      <c r="K36" s="143"/>
+      <c r="M36" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="N36" s="145" t="s">
-        <v>77</v>
-      </c>
-      <c r="O36" s="141" t="s">
-        <v>117</v>
-      </c>
-      <c r="P36" s="143" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q36" s="137" t="s">
-        <v>119</v>
+      <c r="N36" s="127" t="s">
+        <v>76</v>
+      </c>
+      <c r="O36" s="123" t="s">
+        <v>103</v>
+      </c>
+      <c r="P36" s="125" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q36" s="119" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="17.25" customHeight="1">
-      <c r="A37" s="61" t="s">
+      <c r="A37" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="152" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="172"/>
-      <c r="D37" s="153"/>
+      <c r="B37" s="139" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="144"/>
+      <c r="D37" s="140"/>
       <c r="E37" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F37" s="152" t="s">
-        <v>78</v>
-      </c>
-      <c r="G37" s="153"/>
+      <c r="F37" s="139" t="s">
+        <v>77</v>
+      </c>
+      <c r="G37" s="140"/>
       <c r="H37" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" s="146" t="s">
         <v>75</v>
       </c>
-      <c r="I37" s="74" t="s">
+      <c r="K37" s="146"/>
+      <c r="M37" s="130"/>
+      <c r="N37" s="128"/>
+      <c r="O37" s="124"/>
+      <c r="P37" s="126"/>
+      <c r="Q37" s="120"/>
+    </row>
+    <row r="38" spans="1:19" s="111" customFormat="1" ht="15.75">
+      <c r="A38" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="J37" s="178" t="s">
-        <v>76</v>
-      </c>
-      <c r="K37" s="178"/>
-      <c r="M37" s="148"/>
-      <c r="N37" s="146"/>
-      <c r="O37" s="142"/>
-      <c r="P37" s="144"/>
-      <c r="Q37" s="138"/>
-    </row>
-    <row r="38" spans="1:19" s="130" customFormat="1" ht="15.6">
-      <c r="A38" s="127" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="128"/>
-      <c r="C38" s="128"/>
-      <c r="D38" s="128"/>
-      <c r="E38" s="129" t="e">
+      <c r="B38" s="109"/>
+      <c r="C38" s="109"/>
+      <c r="D38" s="109"/>
+      <c r="E38" s="110" t="e">
         <f>+SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="F38" s="128"/>
-      <c r="G38" s="128"/>
-      <c r="I38" s="131" t="e">
+      <c r="F38" s="109"/>
+      <c r="G38" s="109"/>
+      <c r="I38" s="112" t="e">
         <f>+SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="J38" s="132"/>
-      <c r="K38" s="133"/>
-      <c r="L38" s="128"/>
+      <c r="J38" s="113"/>
+      <c r="K38" s="114"/>
+      <c r="L38" s="109"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A39" s="66"/>
+      <c r="A39" s="63"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="43"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="I39" s="94"/>
-      <c r="J39" s="75"/>
-      <c r="K39" s="76"/>
-      <c r="M39" s="162" t="s">
-        <v>120</v>
-      </c>
-      <c r="N39" s="162"/>
-      <c r="O39" s="162"/>
-      <c r="P39" s="166" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q39" s="167"/>
+      <c r="I39" s="83"/>
+      <c r="J39" s="71"/>
+      <c r="K39" s="72"/>
+      <c r="M39" s="152" t="s">
+        <v>106</v>
+      </c>
+      <c r="N39" s="152"/>
+      <c r="O39" s="152"/>
+      <c r="P39" s="156" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q39" s="157"/>
     </row>
     <row r="40" spans="1:19" ht="18.75" customHeight="1">
-      <c r="A40" s="92" t="s">
+      <c r="A40" s="81" t="s">
         <v>53</v>
       </c>
       <c r="B40" s="31"/>
@@ -4236,15 +3654,15 @@
       <c r="H40" s="31"/>
       <c r="I40" s="31"/>
       <c r="J40" s="31"/>
-      <c r="M40" s="162"/>
-      <c r="N40" s="162"/>
-      <c r="O40" s="162"/>
-      <c r="P40" s="168"/>
-      <c r="Q40" s="169"/>
+      <c r="M40" s="152"/>
+      <c r="N40" s="152"/>
+      <c r="O40" s="152"/>
+      <c r="P40" s="158"/>
+      <c r="Q40" s="159"/>
     </row>
     <row r="41" spans="1:19" ht="21">
-      <c r="A41" s="93" t="s">
-        <v>92</v>
+      <c r="A41" s="82" t="s">
+        <v>84</v>
       </c>
       <c r="B41" s="31"/>
       <c r="C41" s="31"/>
@@ -4255,21 +3673,21 @@
       <c r="H41" s="31"/>
       <c r="I41" s="31"/>
       <c r="J41" s="31"/>
-      <c r="M41" s="164" t="s">
-        <v>122</v>
-      </c>
-      <c r="N41" s="165"/>
-      <c r="O41" s="102">
+      <c r="M41" s="154" t="s">
+        <v>108</v>
+      </c>
+      <c r="N41" s="155"/>
+      <c r="O41" s="90" t="e">
         <f>+J31+J30-J32</f>
-        <v>635</v>
-      </c>
-      <c r="P41" s="101" t="s">
-        <v>140</v>
+        <v>#REF!</v>
+      </c>
+      <c r="P41" s="89" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="21">
-      <c r="A42" s="93" t="s">
-        <v>93</v>
+      <c r="A42" s="82" t="s">
+        <v>85</v>
       </c>
       <c r="B42" s="31"/>
       <c r="C42" s="31"/>
@@ -4280,21 +3698,21 @@
       <c r="H42" s="31"/>
       <c r="I42" s="31"/>
       <c r="J42" s="31"/>
-      <c r="M42" s="164" t="s">
-        <v>123</v>
-      </c>
-      <c r="N42" s="165"/>
-      <c r="O42" s="102">
+      <c r="M42" s="154" t="s">
+        <v>109</v>
+      </c>
+      <c r="N42" s="155"/>
+      <c r="O42" s="90" t="e">
         <f>+J33</f>
-        <v>372.00529999999998</v>
-      </c>
-      <c r="P42" s="101" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" ht="18">
-      <c r="A43" s="93" t="s">
-        <v>110</v>
+        <v>#REF!</v>
+      </c>
+      <c r="P42" s="89" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="18.75">
+      <c r="A43" s="82" t="s">
+        <v>96</v>
       </c>
       <c r="B43" s="31"/>
       <c r="C43" s="31"/>
@@ -4306,9 +3724,9 @@
       <c r="I43" s="31"/>
       <c r="J43" s="31"/>
     </row>
-    <row r="44" spans="1:19" ht="18">
-      <c r="A44" s="93" t="s">
-        <v>94</v>
+    <row r="44" spans="1:19" ht="18.75">
+      <c r="A44" s="82" t="s">
+        <v>86</v>
       </c>
       <c r="B44" s="31"/>
       <c r="C44" s="31"/>
@@ -4319,23 +3737,23 @@
       <c r="H44" s="31"/>
       <c r="I44" s="31"/>
       <c r="J44" s="31"/>
-      <c r="M44" s="157" t="s">
-        <v>125</v>
-      </c>
-      <c r="N44" s="157"/>
-      <c r="O44" s="158">
+      <c r="M44" s="147" t="s">
+        <v>111</v>
+      </c>
+      <c r="N44" s="147"/>
+      <c r="O44" s="148" t="e">
         <f>+O41+O42+J14</f>
-        <v>2227.0052999999998</v>
-      </c>
-      <c r="P44" s="160" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q44" s="161"/>
-      <c r="S44" s="163"/>
+        <v>#REF!</v>
+      </c>
+      <c r="P44" s="150" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q44" s="151"/>
+      <c r="S44" s="153"/>
     </row>
     <row r="45" spans="1:19" ht="18.75" customHeight="1">
-      <c r="A45" s="93" t="s">
-        <v>111</v>
+      <c r="A45" s="82" t="s">
+        <v>97</v>
       </c>
       <c r="B45" s="31"/>
       <c r="C45" s="31"/>
@@ -4346,16 +3764,16 @@
       <c r="H45" s="31"/>
       <c r="I45" s="31"/>
       <c r="J45" s="31"/>
-      <c r="M45" s="157"/>
-      <c r="N45" s="157"/>
-      <c r="O45" s="159"/>
-      <c r="P45" s="160"/>
-      <c r="Q45" s="161"/>
-      <c r="S45" s="163"/>
+      <c r="M45" s="147"/>
+      <c r="N45" s="147"/>
+      <c r="O45" s="149"/>
+      <c r="P45" s="150"/>
+      <c r="Q45" s="151"/>
+      <c r="S45" s="153"/>
     </row>
     <row r="46" spans="1:19" ht="18.75" customHeight="1">
-      <c r="A46" s="93" t="s">
-        <v>112</v>
+      <c r="A46" s="82" t="s">
+        <v>98</v>
       </c>
       <c r="B46" s="31"/>
       <c r="C46" s="31"/>
@@ -4366,11 +3784,11 @@
       <c r="H46" s="31"/>
       <c r="I46" s="31"/>
       <c r="J46" s="31"/>
-      <c r="S46" s="163"/>
-    </row>
-    <row r="47" spans="1:19" ht="18">
-      <c r="A47" s="93" t="s">
-        <v>113</v>
+      <c r="S46" s="153"/>
+    </row>
+    <row r="47" spans="1:19" ht="18.75">
+      <c r="A47" s="82" t="s">
+        <v>99</v>
       </c>
       <c r="B47" s="31"/>
       <c r="C47" s="31"/>
@@ -4381,11 +3799,11 @@
       <c r="H47" s="31"/>
       <c r="I47" s="31"/>
       <c r="J47" s="31"/>
-      <c r="S47" s="163"/>
-    </row>
-    <row r="48" spans="1:19" ht="18">
-      <c r="A48" s="93" t="s">
-        <v>109</v>
+      <c r="S47" s="153"/>
+    </row>
+    <row r="48" spans="1:19" ht="18.75">
+      <c r="A48" s="82" t="s">
+        <v>95</v>
       </c>
       <c r="B48" s="31"/>
       <c r="C48" s="31"/>
@@ -4396,7 +3814,7 @@
       <c r="H48" s="31"/>
       <c r="I48" s="31"/>
       <c r="J48" s="31"/>
-      <c r="S48" s="163"/>
+      <c r="S48" s="153"/>
     </row>
     <row r="49" spans="1:19">
       <c r="A49" s="31"/>
@@ -4409,15 +3827,15 @@
       <c r="H49" s="31"/>
       <c r="I49" s="31"/>
       <c r="J49" s="31"/>
-      <c r="S49" s="163"/>
-    </row>
-    <row r="51" spans="1:19" ht="18">
+      <c r="S49" s="153"/>
+    </row>
+    <row r="51" spans="1:19" ht="18.75">
       <c r="H51" s="32"/>
       <c r="I51" s="32"/>
       <c r="J51" s="32"/>
       <c r="K51" s="31"/>
     </row>
-    <row r="52" spans="1:19" ht="18">
+    <row r="52" spans="1:19" ht="18.75">
       <c r="H52" s="32"/>
       <c r="I52" s="32"/>
       <c r="J52" s="32"/>
@@ -4429,22 +3847,22 @@
       <c r="J54" s="40"/>
     </row>
     <row r="56" spans="1:19" ht="21">
-      <c r="A56" s="149" t="s">
+      <c r="A56" s="136" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="149"/>
-      <c r="C56" s="149"/>
-      <c r="D56" s="149"/>
-      <c r="E56" s="149"/>
-      <c r="F56" s="149"/>
-      <c r="G56" s="149"/>
-      <c r="H56" s="149"/>
-      <c r="I56" s="149"/>
-      <c r="J56" s="149"/>
-      <c r="K56" s="149"/>
+      <c r="B56" s="136"/>
+      <c r="C56" s="136"/>
+      <c r="D56" s="136"/>
+      <c r="E56" s="136"/>
+      <c r="F56" s="136"/>
+      <c r="G56" s="136"/>
+      <c r="H56" s="136"/>
+      <c r="I56" s="136"/>
+      <c r="J56" s="136"/>
+      <c r="K56" s="136"/>
     </row>
     <row r="60" spans="1:19">
-      <c r="A60" s="51" t="s">
+      <c r="A60" s="49" t="s">
         <v>47</v>
       </c>
       <c r="B60" s="31"/>
@@ -4452,8 +3870,8 @@
       <c r="D60" s="31"/>
     </row>
     <row r="61" spans="1:19">
-      <c r="A61" s="51" t="s">
-        <v>56</v>
+      <c r="A61" s="49" t="s">
+        <v>55</v>
       </c>
       <c r="B61" s="31"/>
       <c r="C61" s="31"/>
@@ -4461,13 +3879,13 @@
     </row>
     <row r="62" spans="1:19">
       <c r="A62" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C62" s="31"/>
       <c r="D62" s="31"/>
     </row>
     <row r="63" spans="1:19">
-      <c r="A63" s="51" t="s">
+      <c r="A63" s="49" t="s">
         <v>48</v>
       </c>
       <c r="B63" s="31"/>
@@ -4475,8 +3893,8 @@
       <c r="D63" s="31"/>
     </row>
     <row r="64" spans="1:19">
-      <c r="A64" s="51" t="s">
-        <v>58</v>
+      <c r="A64" s="49" t="s">
+        <v>57</v>
       </c>
       <c r="B64" s="31"/>
       <c r="C64" s="31"/>
@@ -4484,13 +3902,13 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C65" s="31"/>
       <c r="D65" s="31"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="51" t="s">
+      <c r="A66" s="49" t="s">
         <v>49</v>
       </c>
       <c r="B66" s="31"/>
@@ -4498,7 +3916,7 @@
       <c r="D66" s="31"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="51" t="s">
+      <c r="A67" s="49" t="s">
         <v>51</v>
       </c>
       <c r="B67" s="31"/>
@@ -4506,39 +3924,39 @@
       <c r="D67" s="31"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="51" t="s">
-        <v>59</v>
+      <c r="A68" s="49" t="s">
+        <v>58</v>
       </c>
       <c r="B68" s="31"/>
       <c r="C68" s="31"/>
       <c r="D68" s="31"/>
     </row>
     <row r="69" spans="1:10">
-      <c r="A69" s="51" t="s">
-        <v>60</v>
+      <c r="A69" s="49" t="s">
+        <v>59</v>
       </c>
       <c r="B69" s="31"/>
       <c r="C69" s="31"/>
       <c r="D69" s="31"/>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="51" t="s">
-        <v>62</v>
+      <c r="A70" s="49" t="s">
+        <v>61</v>
       </c>
       <c r="B70" s="31"/>
       <c r="C70" s="31"/>
       <c r="D70" s="31"/>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="51" t="s">
-        <v>61</v>
+      <c r="A71" s="49" t="s">
+        <v>60</v>
       </c>
       <c r="B71" s="31"/>
       <c r="C71" s="31"/>
       <c r="D71" s="31"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="51" t="s">
+      <c r="A72" s="49" t="s">
         <v>50</v>
       </c>
       <c r="B72" s="31"/>
@@ -4546,16 +3964,16 @@
       <c r="D72" s="31"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="51" t="s">
-        <v>130</v>
+      <c r="A73" s="49" t="s">
+        <v>116</v>
       </c>
       <c r="B73" s="31"/>
       <c r="C73" s="31"/>
       <c r="D73" s="31"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="A77" s="51" t="s">
-        <v>63</v>
+      <c r="A77" s="49" t="s">
+        <v>62</v>
       </c>
       <c r="B77" s="31"/>
       <c r="C77" s="31"/>
@@ -4568,8 +3986,8 @@
       <c r="J77" s="31"/>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="104" t="s">
-        <v>127</v>
+      <c r="A78" s="92" t="s">
+        <v>113</v>
       </c>
       <c r="B78" s="31"/>
       <c r="C78" s="31"/>
@@ -4582,8 +4000,8 @@
       <c r="J78" s="31"/>
     </row>
     <row r="79" spans="1:10">
-      <c r="A79" s="51" t="s">
-        <v>64</v>
+      <c r="A79" s="49" t="s">
+        <v>63</v>
       </c>
       <c r="B79" s="31"/>
       <c r="C79" s="31"/>
@@ -4596,8 +4014,8 @@
       <c r="J79" s="31"/>
     </row>
     <row r="80" spans="1:10">
-      <c r="A80" s="103" t="s">
-        <v>128</v>
+      <c r="A80" s="91" t="s">
+        <v>114</v>
       </c>
       <c r="C80" s="31"/>
       <c r="D80" s="31"/>
@@ -4609,8 +4027,8 @@
       <c r="J80" s="31"/>
     </row>
     <row r="81" spans="1:10">
-      <c r="A81" s="51" t="s">
-        <v>65</v>
+      <c r="A81" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="B81" s="31"/>
       <c r="C81" s="31"/>
@@ -4636,8 +4054,8 @@
       <c r="J82" s="31"/>
     </row>
     <row r="83" spans="1:10">
-      <c r="A83" s="51" t="s">
-        <v>66</v>
+      <c r="A83" s="49" t="s">
+        <v>65</v>
       </c>
       <c r="B83" s="31"/>
       <c r="C83" s="31"/>
@@ -4650,8 +4068,8 @@
       <c r="J83" s="31"/>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" s="51" t="s">
-        <v>67</v>
+      <c r="A84" s="49" t="s">
+        <v>66</v>
       </c>
       <c r="B84" s="31"/>
       <c r="C84" s="31"/>
@@ -4664,8 +4082,8 @@
       <c r="J84" s="31"/>
     </row>
     <row r="85" spans="1:10">
-      <c r="A85" s="51" t="s">
-        <v>68</v>
+      <c r="A85" s="49" t="s">
+        <v>67</v>
       </c>
       <c r="B85" s="31"/>
       <c r="C85" s="31"/>
@@ -4678,8 +4096,8 @@
       <c r="J85" s="31"/>
     </row>
     <row r="86" spans="1:10">
-      <c r="A86" s="51" t="s">
-        <v>69</v>
+      <c r="A86" s="49" t="s">
+        <v>68</v>
       </c>
       <c r="B86" s="31"/>
       <c r="C86" s="31"/>
@@ -4692,8 +4110,8 @@
       <c r="J86" s="31"/>
     </row>
     <row r="87" spans="1:10">
-      <c r="A87" s="51" t="s">
-        <v>129</v>
+      <c r="A87" s="49" t="s">
+        <v>115</v>
       </c>
       <c r="B87" s="31"/>
       <c r="C87" s="31"/>
@@ -4706,16 +4124,16 @@
       <c r="J87" s="31"/>
     </row>
     <row r="91" spans="1:10">
-      <c r="A91" s="51" t="s">
-        <v>83</v>
+      <c r="A91" s="49" t="s">
+        <v>80</v>
       </c>
       <c r="B91" s="31"/>
       <c r="C91" s="31"/>
       <c r="D91" s="31"/>
     </row>
     <row r="92" spans="1:10">
-      <c r="A92" s="51" t="s">
-        <v>84</v>
+      <c r="A92" s="49" t="s">
+        <v>81</v>
       </c>
       <c r="B92" s="31"/>
       <c r="C92" s="31"/>
@@ -4723,7 +4141,7 @@
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="41" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B93" s="31"/>
       <c r="C93" s="31"/>
@@ -4731,21 +4149,21 @@
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="41" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="41" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="2:10">
       <c r="B100" s="41"/>
     </row>
-    <row r="101" spans="2:10" ht="15.6">
+    <row r="101" spans="2:10" ht="15.75">
       <c r="B101" s="42"/>
     </row>
-    <row r="102" spans="2:10" ht="15.6">
+    <row r="102" spans="2:10" ht="15.75">
       <c r="B102" s="42"/>
     </row>
     <row r="104" spans="2:10">
@@ -4766,23 +4184,12 @@
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
     </row>
-    <row r="109" spans="2:10" ht="15.6">
+    <row r="109" spans="2:10" ht="15.75">
       <c r="B109" s="44"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="32">
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="J37:K37"/>
+  <mergeCells count="31">
     <mergeCell ref="M44:N45"/>
     <mergeCell ref="O44:O45"/>
     <mergeCell ref="P44:Q45"/>
@@ -4796,7 +4203,12 @@
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="A36:K36"/>
-    <mergeCell ref="Y11:Y16"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="C3:G4"/>
+    <mergeCell ref="C5:G5"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="Q36:Q37"/>
     <mergeCell ref="M34:Q35"/>
@@ -4804,13 +4216,18 @@
     <mergeCell ref="P36:P37"/>
     <mergeCell ref="N36:N37"/>
     <mergeCell ref="M36:M37"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="COMPROBAR CANTIDAD DE CAJAS" error="Se debe ingresar la cantidad de cajas" sqref="I11" xr:uid="{3C2F8455-5D0D-41B0-BE98-F91BBC4383D3}">
       <formula1>I8&gt;0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11" xr:uid="{543061A4-B74B-4C59-A4B0-2AF20D851021}">
-      <formula1>$W$4:$W$8</formula1>
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
@@ -4826,35 +4243,6 @@
     <ignoredError sqref="I26" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2049" r:id="rId4" name="Button 1">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!fgdfg">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>17</xdr:col>
-                    <xdr:colOff>220980</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>220980</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>18</xdr:col>
-                    <xdr:colOff>464820</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>68580</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -4863,40 +4251,40 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AV54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N24" sqref="J11:N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="2"/>
-    <col min="6" max="6" width="11.33203125" style="2" customWidth="1"/>
-    <col min="7" max="8" width="11.44140625" style="2"/>
-    <col min="9" max="9" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="2"/>
+    <col min="6" max="6" width="11.28515625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" style="2"/>
+    <col min="9" max="9" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="2" customWidth="1"/>
     <col min="11" max="11" width="14" style="2" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="47" width="11.44140625" style="1"/>
+    <col min="12" max="12" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="47" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:47" ht="15" thickBot="1">
-      <c r="B1" s="179" t="s">
+    <row r="1" spans="2:47" ht="15.75" thickBot="1">
+      <c r="B1" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="181"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="162"/>
     </row>
     <row r="2" spans="2:47" s="1" customFormat="1" ht="35.1" customHeight="1">
       <c r="B2" s="43"/>
@@ -4914,8 +4302,8 @@
     <row r="3" spans="2:47" s="1" customFormat="1" ht="23.1" customHeight="1">
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
-      <c r="D3" s="108" t="s">
-        <v>136</v>
+      <c r="D3" s="95" t="s">
+        <v>122</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
@@ -4927,13 +4315,13 @@
       <c r="L3" s="43"/>
     </row>
     <row r="4" spans="2:47">
-      <c r="B4" s="105" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="121">
+      <c r="B4" s="93" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="105">
         <v>1</v>
       </c>
-      <c r="D4" s="108">
+      <c r="D4" s="95">
         <f>COUNT(C4:C4)</f>
         <v>1</v>
       </c>
@@ -4947,51 +4335,51 @@
       <c r="L4" s="43"/>
     </row>
     <row r="5" spans="2:47">
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="121">
+      <c r="C5" s="105">
         <v>1</v>
       </c>
-      <c r="D5" s="108">
+      <c r="D5" s="95">
         <f>SUM(C5:C5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:47">
-      <c r="B6" s="105" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="121">
+      <c r="B6" s="93" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="105">
         <v>23.2</v>
       </c>
-      <c r="D6" s="108">
+      <c r="D6" s="95">
         <f>SUM(C6:C6)</f>
         <v>23.2</v>
       </c>
     </row>
     <row r="7" spans="2:47">
-      <c r="B7" s="105" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="121"/>
+      <c r="B7" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="105"/>
     </row>
     <row r="8" spans="2:47">
-      <c r="B8" s="105" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="121">
+      <c r="B8" s="93" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="105">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="D8" s="108">
+      <c r="D8" s="95">
         <f>SUM(C8:C8)</f>
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="9" spans="2:47" s="1" customFormat="1">
-      <c r="B9" s="110"/>
+      <c r="B9" s="97"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="111"/>
+      <c r="D9" s="98"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -5002,47 +4390,71 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="2:47">
-      <c r="C10" s="109">
+      <c r="C10" s="96">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:47" ht="15" customHeight="1">
-      <c r="B11" s="98" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="98" t="s">
-        <v>142</v>
-      </c>
-      <c r="D11" s="116" t="s">
+      <c r="B11" s="87" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="87" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="101" t="s">
         <v>8</v>
       </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="AQ11"/>
+      <c r="AR11"/>
+      <c r="AS11"/>
+      <c r="AT11"/>
+      <c r="AU11"/>
     </row>
     <row r="12" spans="2:47" ht="15" hidden="1" customHeight="1">
       <c r="B12" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="117">
+      <c r="D12" s="102">
         <f>SUM(C12:C12)</f>
         <v>0</v>
       </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="AQ12"/>
+      <c r="AR12"/>
+      <c r="AS12"/>
+      <c r="AT12"/>
+      <c r="AU12"/>
     </row>
     <row r="13" spans="2:47" ht="15" hidden="1" customHeight="1">
       <c r="B13" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="97"/>
-      <c r="D13" s="118">
+        <v>87</v>
+      </c>
+      <c r="C13" s="86"/>
+      <c r="D13" s="103">
         <f>SUM(C13:C13)</f>
         <v>0</v>
       </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="AQ13"/>
+      <c r="AR13"/>
+      <c r="AS13"/>
+      <c r="AT13"/>
+      <c r="AU13"/>
     </row>
     <row r="14" spans="2:47" ht="15" hidden="1" customHeight="1">
       <c r="B14" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="96"/>
-      <c r="D14" s="119">
+        <v>82</v>
+      </c>
+      <c r="C14" s="85"/>
+      <c r="D14" s="104">
         <f>SUM(C14:C14)</f>
         <v>0</v>
       </c>
@@ -5052,6 +4464,11 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
+      <c r="AL14"/>
+      <c r="AM14"/>
       <c r="AN14"/>
       <c r="AO14"/>
       <c r="AP14"/>
@@ -5062,10 +4479,10 @@
       <c r="AU14"/>
     </row>
     <row r="15" spans="2:47" ht="15" customHeight="1">
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="115">
+      <c r="C15" s="100">
         <v>12.2</v>
       </c>
       <c r="D15" s="1"/>
@@ -5074,17 +4491,18 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
+      <c r="AI15"/>
+      <c r="AJ15"/>
+      <c r="AK15"/>
+      <c r="AL15"/>
+      <c r="AM15"/>
       <c r="AN15"/>
       <c r="AO15"/>
       <c r="AP15"/>
@@ -5095,10 +4513,10 @@
       <c r="AU15"/>
     </row>
     <row r="16" spans="2:47" ht="15" hidden="1" customHeight="1">
-      <c r="B16" s="56" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="57"/>
+      <c r="B16" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="55"/>
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
       <c r="G16" s="2" t="str">
@@ -5107,28 +4525,22 @@
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="J16" s="77">
+        <v>0.4</v>
+      </c>
       <c r="K16" s="3"/>
-      <c r="L16" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="M16" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="N16" s="86">
-        <v>0.6</v>
-      </c>
-      <c r="O16" s="86">
-        <v>0.4</v>
-      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
+      <c r="AI16"/>
+      <c r="AJ16"/>
+      <c r="AK16"/>
+      <c r="AL16"/>
+      <c r="AM16"/>
       <c r="AN16"/>
       <c r="AO16"/>
       <c r="AP16"/>
@@ -5142,10 +4554,10 @@
       <c r="B17" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="114">
+      <c r="C17" s="99">
         <v>100</v>
       </c>
-      <c r="D17" s="117">
+      <c r="D17" s="102">
         <f>SUM(C17:C17)</f>
         <v>100</v>
       </c>
@@ -5154,22 +4566,13 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="7" t="str">
-        <f>'1'!R10</f>
-        <v>NUEVO</v>
-      </c>
-      <c r="L17" s="48">
-        <f>'1'!S10</f>
-        <v>280</v>
-      </c>
-      <c r="M17" s="84">
-        <f>'1'!T10</f>
-        <v>280</v>
-      </c>
-      <c r="N17" s="3">
-        <f>$N$16*L17</f>
-        <v>168</v>
-      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="AI17"/>
+      <c r="AJ17"/>
+      <c r="AK17"/>
+      <c r="AL17"/>
+      <c r="AM17"/>
       <c r="AN17"/>
       <c r="AO17"/>
       <c r="AP17"/>
@@ -5193,22 +4596,13 @@
       </c>
       <c r="E18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="7" t="str">
-        <f>'1'!R11</f>
-        <v>ANTIGUO</v>
-      </c>
-      <c r="L18" s="48">
-        <f>'1'!S11</f>
-        <v>260</v>
-      </c>
-      <c r="M18" s="84">
-        <f>'1'!T11</f>
-        <v>260</v>
-      </c>
-      <c r="N18" s="3">
-        <f t="shared" ref="N18" si="0">$N$16*L18</f>
-        <v>156</v>
-      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="AI18"/>
+      <c r="AJ18"/>
+      <c r="AK18"/>
+      <c r="AL18"/>
+      <c r="AM18"/>
       <c r="AN18"/>
       <c r="AO18"/>
       <c r="AP18"/>
@@ -5219,35 +4613,26 @@
       <c r="AU18"/>
     </row>
     <row r="19" spans="2:48" ht="16.5" hidden="1" customHeight="1">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="59">
+      <c r="C19" s="57">
         <f>(MAX(C15:C16))*C17</f>
         <v>1220</v>
       </c>
-      <c r="D19" s="59">
+      <c r="D19" s="57">
         <f>SUM(C19:C19)</f>
         <v>1220</v>
       </c>
       <c r="E19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="7" t="str">
-        <f>'1'!R12</f>
-        <v>MANUAL</v>
-      </c>
-      <c r="L19" s="48">
-        <f>'1'!S12</f>
-        <v>685</v>
-      </c>
-      <c r="M19" s="84">
-        <f>'1'!T12</f>
-        <v>685</v>
-      </c>
-      <c r="N19" s="3">
-        <f>$N$16*L19</f>
-        <v>411</v>
-      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="AI19"/>
+      <c r="AJ19"/>
+      <c r="AK19"/>
+      <c r="AL19"/>
+      <c r="AM19"/>
       <c r="AN19"/>
       <c r="AO19"/>
       <c r="AP19"/>
@@ -5270,22 +4655,13 @@
       </c>
       <c r="E20" s="30"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="7" t="str">
-        <f>'1'!R13</f>
-        <v>SOCIO</v>
-      </c>
-      <c r="L20" s="48">
-        <f>'1'!S13</f>
-        <v>250</v>
-      </c>
-      <c r="M20" s="84">
-        <f>'1'!T13</f>
-        <v>250</v>
-      </c>
-      <c r="N20" s="3">
-        <f>$N$16*L20</f>
-        <v>150</v>
-      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="AI20"/>
+      <c r="AJ20"/>
+      <c r="AK20"/>
+      <c r="AL20"/>
+      <c r="AM20"/>
       <c r="AN20"/>
       <c r="AO20"/>
       <c r="AP20"/>
@@ -5299,36 +4675,27 @@
       <c r="B21" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="6" t="e">
         <f>$D$21*C20</f>
-        <v>411</v>
-      </c>
-      <c r="D21" s="29">
-        <f>IF(L19=0,IF('1'!E11="NUEVO",'2'!L17*60%,IF('1'!E11="ANTIGUO",'2'!L18*60%,IF('1'!E11="SOCIO",60%*(250*'1'!I11),IF('1'!E11="PILOTO",60%*(250*'1'!I11),IF('2'!L19&gt;0,60%*(250*'1'!I11),IF('1'!E11="MANUAL",60%*(IF('1'!T12&gt;250,('1'!T12*'1'!I11),IF('1'!T12&lt;=250,(250*'1'!I11)))))))))),IF(M19&lt;=250,(250*'1'!I11)*60%,L19*60%))</f>
-        <v>411</v>
-      </c>
-      <c r="E21" s="86"/>
-      <c r="F21" s="183"/>
-      <c r="G21" s="49"/>
+        <v>#REF!</v>
+      </c>
+      <c r="D21" s="29" t="e">
+        <f>IF(#REF!=0,IF('1'!E11="NUEVO",'2'!#REF!*60%,IF('1'!E11="ANTIGUO",'2'!#REF!*60%,IF('1'!E11="SOCIO",60%*(250*'1'!I11),IF('1'!E11="PILOTO",60%*(250*'1'!I11),IF('2'!#REF!&gt;0,60%*(250*'1'!I11),IF('1'!E11="MANUAL",60%*(IF('1'!#REF!&gt;250,('1'!#REF!*'1'!I11),IF('1'!#REF!&lt;=250,(250*'1'!I11)))))))))),IF(#REF!&lt;=250,(250*'1'!I11)*60%,#REF!*60%))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E21" s="77"/>
+      <c r="F21" s="164"/>
+      <c r="G21" s="48"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="7" t="str">
-        <f>'1'!R14</f>
-        <v>PILOTO</v>
-      </c>
-      <c r="L21" s="48">
-        <f>'1'!S14</f>
-        <v>250</v>
-      </c>
-      <c r="M21" s="84">
-        <f>'1'!T14</f>
-        <v>250</v>
-      </c>
-      <c r="N21" s="3">
-        <f>$N$16*L21</f>
-        <v>150</v>
-      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="AI21"/>
+      <c r="AJ21"/>
+      <c r="AK21"/>
+      <c r="AL21"/>
+      <c r="AM21"/>
       <c r="AN21"/>
       <c r="AO21"/>
       <c r="AP21"/>
@@ -5342,32 +4709,27 @@
       <c r="B22" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="18" t="e">
         <f>C18+C21</f>
-        <v>1631</v>
-      </c>
-      <c r="D22" s="18">
+        <v>#REF!</v>
+      </c>
+      <c r="D22" s="18" t="e">
         <f>SUM(C22:C23)</f>
-        <v>3262</v>
+        <v>#REF!</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="183"/>
-      <c r="G22" s="49"/>
+      <c r="F22" s="164"/>
+      <c r="G22" s="48"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="83" t="s">
-        <v>87</v>
-      </c>
-      <c r="J22" s="83"/>
-      <c r="K22" s="50">
-        <f>250*60%</f>
-        <v>150</v>
-      </c>
-      <c r="L22" s="50">
-        <f>250*40%</f>
-        <v>100</v>
-      </c>
-      <c r="M22" s="84"/>
-      <c r="N22" s="3"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="AG22"/>
+      <c r="AH22"/>
+      <c r="AI22"/>
+      <c r="AJ22"/>
+      <c r="AK22"/>
       <c r="AL22"/>
       <c r="AM22"/>
       <c r="AN22"/>
@@ -5380,22 +4742,29 @@
       <c r="AU22"/>
     </row>
     <row r="23" spans="2:48" ht="14.25" hidden="1" customHeight="1">
-      <c r="B23" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="59">
+      <c r="B23" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="57" t="e">
         <f>C19+C21</f>
-        <v>1631</v>
-      </c>
-      <c r="D23" s="59">
+        <v>#REF!</v>
+      </c>
+      <c r="D23" s="57" t="e">
         <f>SUM(C23:C23)</f>
-        <v>1631</v>
+        <v>#REF!</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="G23" s="49"/>
+      <c r="G23" s="48"/>
       <c r="H23" s="1"/>
       <c r="I23" s="30"/>
       <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="AI23"/>
+      <c r="AJ23"/>
+      <c r="AK23"/>
+      <c r="AL23"/>
+      <c r="AM23"/>
       <c r="AN23"/>
       <c r="AO23"/>
       <c r="AP23"/>
@@ -5418,12 +4787,17 @@
         <v>50</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="G24" s="49"/>
+      <c r="G24" s="48"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
+      <c r="AI24"/>
+      <c r="AJ24"/>
+      <c r="AK24"/>
+      <c r="AL24"/>
+      <c r="AM24"/>
       <c r="AN24"/>
       <c r="AO24"/>
       <c r="AP24"/>
@@ -5437,16 +4811,16 @@
       <c r="B25" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="18">
-        <f t="shared" ref="C25" si="1">C22+C24</f>
-        <v>1681</v>
-      </c>
-      <c r="D25" s="18">
+      <c r="C25" s="18" t="e">
+        <f t="shared" ref="C25" si="0">C22+C24</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D25" s="18" t="e">
         <f>SUM(C25:C26)</f>
-        <v>3362</v>
+        <v>#REF!</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="G25" s="49"/>
+      <c r="G25" s="48"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -5462,56 +4836,59 @@
       <c r="AU25"/>
     </row>
     <row r="26" spans="2:48" ht="18.75" hidden="1" customHeight="1">
-      <c r="B26" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="59">
+      <c r="B26" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="57" t="e">
         <f>C23+C24</f>
-        <v>1681</v>
-      </c>
-      <c r="D26" s="59">
+        <v>#REF!</v>
+      </c>
+      <c r="D26" s="57" t="e">
         <f>SUM(C26:C26)</f>
-        <v>1681</v>
-      </c>
-      <c r="G26" s="49"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G26" s="48"/>
     </row>
     <row r="27" spans="2:48">
-      <c r="G27" s="49"/>
+      <c r="G27" s="48"/>
     </row>
     <row r="28" spans="2:48">
-      <c r="B28" s="185" t="s">
+      <c r="B28" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="185"/>
-      <c r="D28" s="185"/>
-      <c r="E28" s="185"/>
-      <c r="F28" s="185"/>
-      <c r="G28" s="185"/>
-      <c r="H28" s="185"/>
-      <c r="I28" s="185"/>
-      <c r="J28" s="185"/>
-      <c r="K28" s="185"/>
-      <c r="L28" s="185"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="166"/>
+      <c r="L28" s="166"/>
     </row>
     <row r="30" spans="2:48">
-      <c r="C30" s="52"/>
+      <c r="C30" s="50"/>
       <c r="M30" s="2"/>
       <c r="AV30" s="1"/>
     </row>
     <row r="31" spans="2:48">
-      <c r="B31" s="53" t="s">
+      <c r="B31" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="54">
+      <c r="C31" s="52">
         <f>C17*C30</f>
         <v>0</v>
       </c>
-      <c r="D31" s="54">
+      <c r="D31" s="52">
         <f>SUM(C31:C31)</f>
         <v>0</v>
       </c>
       <c r="M31" s="2"/>
       <c r="AV31" s="1"/>
+    </row>
+    <row r="32" spans="2:48">
+      <c r="G32" s="109"/>
     </row>
     <row r="33" spans="1:47">
       <c r="C33" s="11">
@@ -5523,8 +4900,8 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="184"/>
-      <c r="I33" s="184"/>
+      <c r="H33" s="165"/>
+      <c r="I33" s="165"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -5541,19 +4918,19 @@
       <c r="B34" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="6" t="e">
         <f>MAX(C25:C26)*C33</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="10">
+        <v>#REF!</v>
+      </c>
+      <c r="D34" s="10" t="e">
         <f>SUM(C34:C34)</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="184"/>
-      <c r="I34" s="184"/>
+      <c r="H34" s="165"/>
+      <c r="I34" s="165"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -5571,13 +4948,13 @@
       <c r="B35" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="13">
+      <c r="C35" s="13" t="e">
         <f>((MAX(C25:C26))+C34)*16%</f>
-        <v>268.95999999999998</v>
-      </c>
-      <c r="D35" s="10">
+        <v>#REF!</v>
+      </c>
+      <c r="D35" s="10" t="e">
         <f>SUM(C35:C35)</f>
-        <v>268.95999999999998</v>
+        <v>#REF!</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -5620,13 +4997,13 @@
       <c r="B36" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="15">
-        <f t="shared" ref="C36" si="2">((MAX(C25:C26))+C34)*2%</f>
-        <v>33.619999999999997</v>
-      </c>
-      <c r="D36" s="10">
+      <c r="C36" s="15" t="e">
+        <f t="shared" ref="C36" si="1">((MAX(C25:C26))+C34)*2%</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D36" s="10" t="e">
         <f>SUM(C36:C36)</f>
-        <v>33.619999999999997</v>
+        <v>#REF!</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
@@ -5669,13 +5046,13 @@
       <c r="B37" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="15">
-        <f t="shared" ref="C37" si="3">(C25+C34+C35+C36)*3.5%</f>
-        <v>69.425300000000007</v>
-      </c>
-      <c r="D37" s="10">
+      <c r="C37" s="15" t="e">
+        <f t="shared" ref="C37" si="2">(C25+C34+C35+C36)*3.5%</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D37" s="10" t="e">
         <f>SUM(C37:C37)</f>
-        <v>69.425300000000007</v>
+        <v>#REF!</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
@@ -5717,13 +5094,13 @@
       <c r="B38" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="20">
-        <f t="shared" ref="C38" si="4">SUM(C34:C37)</f>
-        <v>372.00529999999998</v>
-      </c>
-      <c r="D38" s="18">
+      <c r="C38" s="20" t="e">
+        <f t="shared" ref="C38" si="3">SUM(C34:C37)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D38" s="18" t="e">
         <f>SUM(C38:C38)</f>
-        <v>372.00529999999998</v>
+        <v>#REF!</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -5759,19 +5136,19 @@
       </c>
     </row>
     <row r="42" spans="1:47">
-      <c r="B42" s="182" t="s">
+      <c r="B42" s="163" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="182"/>
-      <c r="D42" s="182"/>
-      <c r="E42" s="182"/>
-      <c r="F42" s="182"/>
-      <c r="G42" s="182"/>
-      <c r="H42" s="182"/>
-      <c r="I42" s="182"/>
-      <c r="J42" s="182"/>
-      <c r="K42" s="182"/>
-      <c r="L42" s="182"/>
+      <c r="C42" s="163"/>
+      <c r="D42" s="163"/>
+      <c r="E42" s="163"/>
+      <c r="F42" s="163"/>
+      <c r="G42" s="163"/>
+      <c r="H42" s="163"/>
+      <c r="I42" s="163"/>
+      <c r="J42" s="163"/>
+      <c r="K42" s="163"/>
+      <c r="L42" s="163"/>
     </row>
     <row r="44" spans="1:47">
       <c r="C44" s="21">
@@ -5802,15 +5179,15 @@
       <c r="B45" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="23">
+      <c r="C45" s="23" t="e">
         <f>$D$45*C44</f>
-        <v>274</v>
-      </c>
-      <c r="D45" s="29">
-        <f>IF(L19=0,IF('1'!E11="NUEVO",'2'!L17*40%,IF('1'!E11="ANTIGUO",'2'!L18*40%,IF('1'!E11="SOCIO",40%*(250*'1'!I11),IF('1'!E11="PILOTO",40%*(250*'1'!I11),IF('2'!L19&gt;0,40%*(250*'1'!I11),IF('1'!E11="MANUAL",40%*(IF('1'!T12&gt;250,('1'!T12*'1'!I11),IF('1'!T12&lt;=250,(250*'1'!I11)))))))))),IF(M19&lt;=250,(250*'1'!I11)*40%,L19*40%))</f>
-        <v>274</v>
-      </c>
-      <c r="E45" s="86"/>
+        <v>#REF!</v>
+      </c>
+      <c r="D45" s="29" t="e">
+        <f>IF(#REF!=0,IF('1'!E11="NUEVO",'2'!#REF!*40%,IF('1'!E11="ANTIGUO",'2'!#REF!*40%,IF('1'!E11="SOCIO",40%*(250*'1'!I11),IF('1'!E11="PILOTO",40%*(250*'1'!I11),IF('2'!#REF!&gt;0,40%*(250*'1'!I11),IF('1'!E11="MANUAL",40%*(IF('1'!#REF!&gt;250,('1'!#REF!*'1'!I11),IF('1'!#REF!&lt;=250,(250*'1'!I11)))))))))),IF(#REF!&lt;=250,(250*'1'!I11)*40%,#REF!*40%))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E45" s="77"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -5835,26 +5212,26 @@
       <c r="G46" s="4"/>
     </row>
     <row r="48" spans="1:47">
-      <c r="B48" s="99" t="s">
+      <c r="B48" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="99"/>
-      <c r="D48" s="99"/>
-      <c r="E48" s="99"/>
-      <c r="F48" s="99"/>
-      <c r="G48" s="99"/>
-      <c r="H48" s="99"/>
-      <c r="I48" s="99"/>
-      <c r="J48" s="99"/>
-      <c r="K48" s="99"/>
-      <c r="L48" s="99"/>
+      <c r="C48" s="88"/>
+      <c r="D48" s="88"/>
+      <c r="E48" s="88"/>
+      <c r="F48" s="88"/>
+      <c r="G48" s="88"/>
+      <c r="H48" s="88"/>
+      <c r="I48" s="88"/>
+      <c r="J48" s="88"/>
+      <c r="K48" s="88"/>
+      <c r="L48" s="88"/>
     </row>
     <row r="50" spans="2:47">
       <c r="B50" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C50" s="7" t="str">
-        <f t="shared" ref="C50" si="5">C11</f>
+        <f t="shared" ref="C50" si="4">C11</f>
         <v>BASE DE LAMPARA LED</v>
       </c>
       <c r="E50" s="1"/>
@@ -5878,13 +5255,13 @@
       <c r="B51" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="23">
+      <c r="C51" s="23" t="e">
         <f>C18+C38+C31+'2'!C20*('1'!$J$31)</f>
-        <v>1642.0053</v>
-      </c>
-      <c r="D51" s="23">
+        <v>#REF!</v>
+      </c>
+      <c r="D51" s="23" t="e">
         <f>SUM(C51:C51)</f>
-        <v>1642.0053</v>
+        <v>#REF!</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -5932,9 +5309,9 @@
       <c r="B53" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="23">
-        <f t="shared" ref="C53" si="6">C51/C52</f>
-        <v>16.420052999999999</v>
+      <c r="C53" s="23" t="e">
+        <f t="shared" ref="C53" si="5">C51/C52</f>
+        <v>#REF!</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -5957,9 +5334,9 @@
       <c r="B54" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="26">
+      <c r="C54" s="26" t="e">
         <f>C53*$P$40</f>
-        <v>60.754196100000001</v>
+        <v>#REF!</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -5992,6 +5369,5 @@
   <cellWatches>
     <cellWatch r="D38"/>
   </cellWatches>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>